<commit_message>
Add baptismal date to confirmation detail
</commit_message>
<xml_diff>
--- a/public/forms/confirmation-format.xlsx
+++ b/public/forms/confirmation-format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\church-mis\public\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42850E6A-262A-46C5-BE6F-C161486E9207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8594510C-AB4E-4316-9CE9-1BC01ADCE606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2AF45597-10AB-400D-B240-38F312BD0E22}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Leslie Panganiban</t>
+  </si>
+  <si>
+    <t>Baptismal Date</t>
   </si>
 </sst>
 </file>
@@ -161,7 +164,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
+      <xdr:colOff>209550</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>985345</xdr:rowOff>
     </xdr:to>
@@ -496,22 +499,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{670E7318-4698-4C2F-93B7-823947330421}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" style="3" customWidth="1"/>
-    <col min="3" max="6" width="22.85546875" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="34.85546875" customWidth="1"/>
+    <col min="2" max="3" width="20.5703125" style="3" customWidth="1"/>
+    <col min="4" max="7" width="22.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -520,8 +523,9 @@
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -529,107 +533,119 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="1"/>
       <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3">
         <v>34899</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3">
+        <v>45352</v>
+      </c>
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="4">
+      <c r="H3" s="4">
         <v>9062268483</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="3">
         <v>34899</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3">
+        <v>45353</v>
+      </c>
+      <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="4">
+      <c r="H4" s="4">
         <v>9062268483</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="3">
         <v>34899</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3">
+        <v>45354</v>
+      </c>
+      <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>14</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="4">
+      <c r="H5" s="4">
         <v>9062268483</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>